<commit_message>
reupload after crush HDD
</commit_message>
<xml_diff>
--- a/sneakers.xlsx
+++ b/sneakers.xlsx
@@ -442,41 +442,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow 5000</t>
+          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>21.490.₽</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/676/296_296_2/th9pk1w9xbr4349gsjsu58xpeqe305xa.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/046/296_296_2/nfeq0doxq94c7x5jnrrzyrrnckknwqqq.JPG </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow 6000</t>
+          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>21.490.₽</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7f5/296_296_2/fl6dru8cv1ax0w0s3woiegss1e03537y.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d95/296_296_2/4j1dbggpomuzyep5g205k53ctzw49ss4.JPG </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow 6000</t>
+          <t>Кроссовки Saucony Shadow 5000</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -486,7 +486,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/008/296_296_2/v2vf86dvtzc50bhbakhk1wgmkpm0d5qw.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/676/296_296_2/th9pk1w9xbr4349gsjsu58xpeqe305xa.jpg </t>
         </is>
       </c>
     </row>
@@ -503,7 +503,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a13/296_296_2/ylzxac88e18cbc6fdb14lv9pjeos90io.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7f5/296_296_2/fl6dru8cv1ax0w0s3woiegss1e03537y.JPG </t>
         </is>
       </c>
     </row>
@@ -515,131 +515,131 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>18.900.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae3/296_296_2/lk7cjjtlwenbsnaz8lupawb1gg92u89d.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/008/296_296_2/v2vf86dvtzc50bhbakhk1wgmkpm0d5qw.JPG </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Jazz 81</t>
+          <t>Кроссовки Saucony Shadow 6000</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>13.900.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/346/296_296_2/m9br8zd2ifkgceufr7wgb57ijdvev81w.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a13/296_296_2/ylzxac88e18cbc6fdb14lv9pjeos90io.JPG </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow Original</t>
+          <t>Кроссовки Saucony Shadow 6000</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14.400.₽</t>
+          <t>18.900.₽</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/88a/296_296_2/xq8k79ozpfybxo7zfftkj8kbxchw2u4g.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae3/296_296_2/lk7cjjtlwenbsnaz8lupawb1gg92u89d.JPG </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony 3D Grid Hurricane</t>
+          <t>Кроссовки Saucony Jazz 81</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>17.990.₽</t>
+          <t>13.900.₽</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae1/296_296_2/d8aurlto7sc2me0heb4jmwgbuapecfwl.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/346/296_296_2/m9br8zd2ifkgceufr7wgb57ijdvev81w.JPG </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Zoom Spiridon Cage 2</t>
+          <t>Кроссовки Saucony Shadow Original</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>14.400.₽</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5e7/296_296_2/t10f9zno250mzry3e6tzpporrk19pxer.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/88a/296_296_2/xq8k79ozpfybxo7zfftkj8kbxchw2u4g.JPG </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Space Hippie 01</t>
+          <t>Кроссовки Saucony 3D Grid Hurricane</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>12.990.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/4f2/296_296_2/12uei3kk0sftwwxxc6era6nh0bhmk5te.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae1/296_296_2/d8aurlto7sc2me0heb4jmwgbuapecfwl.JPG </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Dunk Low Retro</t>
+          <t>Кроссовки Nike Air Zoom Spiridon Cage 2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c05/296_296_2/vu9m6mnwmeqa58ky1nmd4cgp1sjl92ld.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5e7/296_296_2/t10f9zno250mzry3e6tzpporrk19pxer.JPG </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 '07 LV8</t>
+          <t>Кроссовки Nike Space Hippie 01</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>12.990.₽</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/663/296_296_2/tqg36ogeibeejpt48jkcvphr16k4pwgm.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/4f2/296_296_2/12uei3kk0sftwwxxc6era6nh0bhmk5te.JPG </t>
         </is>
       </c>
     </row>
@@ -748,51 +748,51 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 Mid (GS)</t>
+          <t>Кроссовки Nike WMNS Air Force 1 High OG QS</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16.490.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/098/296_296_2/es3ww7bfe6eyxjbjx7nk1wdbh19ew4ug.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bb3/296_296_2/m2t337wcsv54e89oqpij9k29iutwb2qu.JPG </t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 High OG QS</t>
+          <t>Кроссовки Jordan WMNS 1 Mid</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>21.990.₽</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bb3/296_296_2/m2t337wcsv54e89oqpij9k29iutwb2qu.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/274/296_296_2/27443d085d6096b2f951a9d40f4c669c.jpg </t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan WMNS 1 Mid</t>
+          <t>Кроссовки New Balance 574</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/274/296_296_2/27443d085d6096b2f951a9d40f4c669c.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fe1/296_296_2/hxbjvb19wez1ka68d1l20c6iu3rv4esj.JPG </t>
         </is>
       </c>
     </row>
@@ -809,126 +809,126 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fe1/296_296_2/hxbjvb19wez1ka68d1l20c6iu3rv4esj.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c7d/296_296_2/u2f3uguex22a6i36dhd8nfrgm9gkd1kd.JPG </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 574</t>
+          <t>Кроссовки Nike Dunk Low Retro</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c7d/296_296_2/u2f3uguex22a6i36dhd8nfrgm9gkd1kd.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/57d/296_296_2/57d1ef7f67047d6aa549245f00fd59a0.jpg </t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Dunk Low Retro</t>
+          <t>Кроссовки Mizuno Wave Rider 1</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>18.490.₽</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/57d/296_296_2/57d1ef7f67047d6aa549245f00fd59a0.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e7d/296_296_2/d2kcnhpvwxoqjkz029be3ybk5b5bf0fn.JPG </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Wave Rider 1</t>
+          <t>Кроссовки Mizuno Contender</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>18.490.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e7d/296_296_2/d2kcnhpvwxoqjkz029be3ybk5b5bf0fn.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b8/296_296_2/fo0qlr2vot0iycmapaark2vd7a43mm5g.JPG </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Contender</t>
+          <t>Кроссовки PUMA RS-X Hi</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>15.990.₽</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b8/296_296_2/fo0qlr2vot0iycmapaark2vd7a43mm5g.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c51/296_296_2/4bpayspdv4t889e9h2xyu5nxfns88p1u.jpg </t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA RS-X Hi</t>
+          <t>Кроссовки Nike WMNS Air Force 1 Shadow</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>15.990.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c51/296_296_2/4bpayspdv4t889e9h2xyu5nxfns88p1u.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cea/296_296_2/ypo43ssbkl0lb9h9pftwjye1cjxahs3c.JPG </t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 Shadow</t>
+          <t>Кроссовки New Balance 2002R</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>22.990.₽</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cea/296_296_2/ypo43ssbkl0lb9h9pftwjye1cjxahs3c.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e4d/296_296_2/e4d5b3596faee2bd476db4f711f10cd0.jpg </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Wave Rider 10</t>
+          <t>Кроссовки PUMA Slipstream Hi Xtreme Cordura</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>14.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/84f/296_296_2/9drxj66ie39iw0mssxn485fxkjn2h3ia.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e7c/296_296_2/tnk0n8vldc4nya4fal6nd6eo1aquj1p1.JPG </t>
         </is>
       </c>
     </row>
@@ -945,14 +945,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e7c/296_296_2/tnk0n8vldc4nya4fal6nd6eo1aquj1p1.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cef/296_296_2/obiyh0ljm0v21pz2pp2nxdxv8p6ms6p2.JPG </t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Hi Xtreme Cordura</t>
+          <t>Кроссовки PUMA Slipstream Hi Xtreme</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -962,41 +962,41 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cef/296_296_2/obiyh0ljm0v21pz2pp2nxdxv8p6ms6p2.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/72b/296_296_2/j1zj2c90bn9qjq4xx157njfg7fwzx8e1.JPG </t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Hi Xtreme</t>
+          <t>Кроссовки ASICS Gel-1130</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>14.990.₽</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/72b/296_296_2/j1zj2c90bn9qjq4xx157njfg7fwzx8e1.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cfb/296_296_2/k2wlfll8x9rlxb1jz9tp0b8laq83ssw6.JPG </t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Кроссовки ASICS Gel-1130</t>
+          <t>Кроссовки ASICS Gel-Kayano 14</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>14.990.₽</t>
+          <t>21.990.₽</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cfb/296_296_2/k2wlfll8x9rlxb1jz9tp0b8laq83ssw6.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/822/296_296_2/n8jmzs7zactks5jg11yq4aaq2auup486.JPG </t>
         </is>
       </c>
     </row>
@@ -1105,187 +1105,187 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Max 97</t>
+          <t>Кроссовки Nike WMNS Air Vapormax 2021 FK</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>20.990.₽</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/23d/296_296_2/9r8xi8fe61imxhxzlgkhfkzfn6i4etkd.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0bd/296_296_2/z50ayuan1ca9kh9x2u0z5soyku823gf1.JPG </t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Vapormax 2021 FK</t>
+          <t>Кроссовки Nike Air Force 1 Crater Flyknit NN</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>20.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0bd/296_296_2/z50ayuan1ca9kh9x2u0z5soyku823gf1.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0c5/296_296_2/2d8fok2200a1b6zimxx29ttp6p1n22zs.JPG </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 Crater Flyknit NN</t>
+          <t xml:space="preserve">Кроссовки Jordan 1 Retro High Utility SP </t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>24.990.₽</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0c5/296_296_2/2d8fok2200a1b6zimxx29ttp6p1n22zs.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9c2/296_296_2/sko9wgbqdrwub5gikyu2to2dg6dn4ihl.JPG </t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кроссовки Jordan 1 Retro High Utility SP </t>
+          <t>Кроссовки Nike ZoomX Vaporfly</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>24.990.₽</t>
+          <t>31.990.₽</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9c2/296_296_2/sko9wgbqdrwub5gikyu2to2dg6dn4ihl.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a7d/296_296_2/3shqdya6m5ag7frpr4zbt60j0848d46f.JPG </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Кроссовки Nike ZoomX Vaporfly</t>
+          <t>Кроссовки Jordan 1 ZOOM AIR CMFT</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>31.990.₽</t>
+          <t>21.990.₽</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a7d/296_296_2/3shqdya6m5ag7frpr4zbt60j0848d46f.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/801/296_296_2/abnpm41gq4kb5d4rwl567px608bfqxy5.JPG </t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 ZOOM AIR CMFT</t>
+          <t>Кроссовки Nike Air Max SC</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>21.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/801/296_296_2/abnpm41gq4kb5d4rwl567px608bfqxy5.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/045/296_296_2/hda9q0wyrbhni95yqjerddwjzkvcsyi9.JPG </t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Max SC</t>
+          <t>Кроссовки Li-Ning Wave Pro</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>10.490.₽</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/045/296_296_2/hda9q0wyrbhni95yqjerddwjzkvcsyi9.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/822/296_296_2/r4pt14oz9i2g99aslvj4kjvmyxaohosr.JPG </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Кроссовки Li-Ning Wave Pro</t>
+          <t>Кроссовки Li-Ning Wave Pro SE</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>10.490.₽</t>
+          <t>11.590.₽</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/822/296_296_2/r4pt14oz9i2g99aslvj4kjvmyxaohosr.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0e4/296_296_2/baf4l4w7rtki2j50r36bvmtnxszrt14e.JPG </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Кроссовки Li-Ning Wave Pro SE</t>
+          <t>Кроссовки Nike ACG Moc 3.5</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>11.590.₽</t>
+          <t>11.990.₽</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0e4/296_296_2/baf4l4w7rtki2j50r36bvmtnxszrt14e.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/60f/296_296_2/xbv1uldhbv70yh7k990nhwv25643u62k.JPG </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Кроссовки Nike ACG Moc 3.5</t>
+          <t>Кроссовки Nike Air Force 1 LE (GS)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>11.990.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/60f/296_296_2/xbv1uldhbv70yh7k990nhwv25643u62k.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d5e/296_296_2/d5ebbacaa03f8ce6957fbab928d42eee.jpg </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 LE (GS)</t>
+          <t>Кроссовки Jordan WMNS 1 Acclimate</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>21.000.₽</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d5e/296_296_2/d5ebbacaa03f8ce6957fbab928d42eee.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/510/296_296_2/3mencgkhigsy0rp4az1030oxwmt3zsdu.JPG </t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/510/296_296_2/3mencgkhigsy0rp4az1030oxwmt3zsdu.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fa7/296_296_2/6u4o87au7d6veyqbjx5lu168ckgspwxx.JPG </t>
         </is>
       </c>
     </row>
@@ -1319,286 +1319,286 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fa7/296_296_2/6u4o87au7d6veyqbjx5lu168ckgspwxx.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a1c/296_296_2/yo8n34xfiwo8s6arqiln0owrq0i80iba.JPG </t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan WMNS 1 Acclimate</t>
+          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>21.000.₽</t>
+          <t>20.000.₽</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a1c/296_296_2/yo8n34xfiwo8s6arqiln0owrq0i80iba.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fcf/296_296_2/fsokqf6rdx7ohynq1ynvzy72iub42dc6.JPG </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
+          <t>Кроссовки Nike Air Force 1 '07</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>20.000.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fcf/296_296_2/fsokqf6rdx7ohynq1ynvzy72iub42dc6.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/2d5/296_296_2/1q2tek49apdlbtc6ggsj3h39zono0giv.JPG </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 '07</t>
+          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/2d5/296_296_2/1q2tek49apdlbtc6ggsj3h39zono0giv.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a3a/296_296_2/nmivl13a5m0cy447mnyt9xy2c6i3d13w.JPG </t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
+          <t>Кроссовки Nike Air Force 1 '07</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a3a/296_296_2/nmivl13a5m0cy447mnyt9xy2c6i3d13w.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b2/296_296_2/fpbnqjfiyl6u8yvf42agnoknzgk1yg0m.JPG </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 '07</t>
+          <t>Кроссовки Nike Dunk Low Retro PRM</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>20.990.₽</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b2/296_296_2/fpbnqjfiyl6u8yvf42agnoknzgk1yg0m.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/483/296_296_2/5ckjgio7rfyerf2s9ek5y6wuba9a0h01.JPG </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Dunk Low Retro PRM</t>
+          <t>Кроссовки Nike WMNS Dunk Low LX</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>20.990.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/483/296_296_2/5ckjgio7rfyerf2s9ek5y6wuba9a0h01.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/47f/296_296_2/tbrur5tjllknu907e8r62eadzohmecdq.JPG </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Dunk Low LX</t>
+          <t>Кроссовки Nike ACG Mountain Fly 2 Low</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>17.990.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/47f/296_296_2/tbrur5tjllknu907e8r62eadzohmecdq.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/da4/296_296_2/o1swj5riifulqv62i7x7yag0esds6tlb.JPG </t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Кроссовки Nike ACG Mountain Fly 2 Low</t>
+          <t>Кроссовки PUMA Slipstream Suede</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>10.190.₽</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/da4/296_296_2/o1swj5riifulqv62i7x7yag0esds6tlb.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1e7/296_296_2/luq43cv83p432jwj3zolpe8ttvqronqh.JPG </t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Suede</t>
+          <t>Кроссовки Diadora N9000 Rally Giulietta Itali</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>10.190.₽</t>
+          <t>26.790.₽</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1e7/296_296_2/luq43cv83p432jwj3zolpe8ttvqronqh.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/998/296_296_2/prlbuactqqt6km4sn7r8snysz9sl53ik.JPG </t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N9000 Rally Giulietta Itali</t>
+          <t>Кроссовки Diadora B.560 Used</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>26.790.₽</t>
+          <t>24.490.₽</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/998/296_296_2/prlbuactqqt6km4sn7r8snysz9sl53ik.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c64/296_296_2/c0fqcfk3ssgfnrxll76psxi33uyvn813.JPG </t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora B.560 Used</t>
+          <t>Кроссовки Diadora B.56 Icona</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>24.490.₽</t>
+          <t>12.190.₽</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c64/296_296_2/c0fqcfk3ssgfnrxll76psxi33uyvn813.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/155/296_296_2/tjwnrwrow86mujignvqhapmy0wdvc56f.JPG </t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora B.56 Icona</t>
+          <t>Кроссовки Diadora Magic Basket Low Suede Leather</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>12.190.₽</t>
+          <t>12.590.₽</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/155/296_296_2/tjwnrwrow86mujignvqhapmy0wdvc56f.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/85a/296_296_2/ifh2xgzc3lkvi4l919fjdgqbvgmkf1sn.JPG </t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora Magic Basket Low Suede Leather</t>
+          <t>Кроссовки Diadora N.92 Advance</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>12.590.₽</t>
+          <t>10.490.₽</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/85a/296_296_2/ifh2xgzc3lkvi4l919fjdgqbvgmkf1sn.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d00/296_296_2/2o731rmeir6av9x2i70txdm46dqoz0xx.JPG </t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N.92 Advance</t>
+          <t>Кроссовки Diadora N902 Hairy Suede</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10.490.₽</t>
+          <t>11.190.₽</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d00/296_296_2/2o731rmeir6av9x2i70txdm46dqoz0xx.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/3da/296_296_2/91pw2xy60tn25sp2t0qse7leuzppif85.JPG </t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N902 Hairy Suede</t>
+          <t>Кроссовки Diadora N902</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>11.190.₽</t>
+          <t>14.890.₽</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/3da/296_296_2/91pw2xy60tn25sp2t0qse7leuzppif85.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1c9/296_296_2/wej9c1s9undfcvlxl3jwoh6kb6funvxu.JPG </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N902</t>
+          <t>Кроссовки Diadora V7000 Winter</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>14.890.₽</t>
+          <t>14.190.₽</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1c9/296_296_2/wej9c1s9undfcvlxl3jwoh6kb6funvxu.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae4/296_296_2/fnt7nsc3jupi22ue464cxbp9jmwbqq20.jpg </t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora V7000 Winter</t>
+          <t xml:space="preserve">Кроссовки Diadora V7000 Winter </t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1608,24 +1608,24 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae4/296_296_2/fnt7nsc3jupi22ue464cxbp9jmwbqq20.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e69/296_296_2/3urr2nxltn6nrnog4mqhliulquiy7p97.JPG </t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кроссовки Diadora V7000 Winter </t>
+          <t>Кроссовки Diadora N9002 Winter</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>14.190.₽</t>
+          <t>16.390.₽</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e69/296_296_2/3urr2nxltn6nrnog4mqhliulquiy7p97.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e65/296_296_2/4fe7jsy4klih38kzyqe8labyt2wys8ar.JPG </t>
         </is>
       </c>
     </row>
@@ -1642,75 +1642,75 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e65/296_296_2/4fe7jsy4klih38kzyqe8labyt2wys8ar.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/688/296_296_2/47achzhjvpul8jbeyn5pf26qubzwmuf8.JPG </t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N9002 Winter</t>
+          <t>Кроссовки Mizuno Contender</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16.390.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/688/296_296_2/47achzhjvpul8jbeyn5pf26qubzwmuf8.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b56/296_296_2/ce779p9n380lfnw58yk8b1han4ftjbwc.JPG </t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Contender</t>
+          <t>Кроссовки Mizuno Wave Rider 10</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>20.990.₽</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b56/296_296_2/ce779p9n380lfnw58yk8b1han4ftjbwc.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/2a8/296_296_2/2f7yvxz0a9pvzapkmhkca97lgawh4amx.JPG </t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Wave Rider 10</t>
+          <t>Кроссовки Mizuno City Wind</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>20.990.₽</t>
+          <t>14.990.₽</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/2a8/296_296_2/2f7yvxz0a9pvzapkmhkca97lgawh4amx.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c8e/296_296_2/k9sjc434r3qmn6my5dwwjz325mwxzeh0.JPG </t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno City Wind</t>
+          <t>Кроссовки Mizuno Wave Mujin TL GTX</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>14.990.₽</t>
+          <t>24.990.₽</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c8e/296_296_2/k9sjc434r3qmn6my5dwwjz325mwxzeh0.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/396/296_296_2/4a57232ajluzciuvomuvow2xc4p4vzn2.JPG </t>
         </is>
       </c>
     </row>
@@ -1727,143 +1727,143 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/396/296_296_2/4a57232ajluzciuvomuvow2xc4p4vzn2.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/f37/296_296_2/9qo14d029kjb0nri86pwhug41db3wjmg.JPG </t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Wave Mujin TL GTX</t>
+          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>24.990.₽</t>
+          <t>20.000.₽</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/f37/296_296_2/9qo14d029kjb0nri86pwhug41db3wjmg.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1d0/296_296_2/5y0m14acunvwl6ch0y16y4c7vytgvayd.jpg </t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 '07</t>
+          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>21.000.₽</t>
+          <t>24.000.₽</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8b3/296_296_2/6b7w8lgab9521w5w9e9yh4xq8ehrf55o.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/955/296_296_2/04i3rsojwt4rs4hxrhwbzawyj52zyti3.jpg </t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
+          <t>Кроссовки Reebok Club C Mid II Revenge Vintage</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>20.000.₽</t>
+          <t>11.590.₽</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1d0/296_296_2/5y0m14acunvwl6ch0y16y4c7vytgvayd.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1f3/296_296_2/erhqtcmroqwyw6ootl4q2bp4soqpbljx.JPG </t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
+          <t>Кроссовки Reebok Classic Leather Mid GTX-Thin</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>24.000.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/955/296_296_2/04i3rsojwt4rs4hxrhwbzawyj52zyti3.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/79c/296_296_2/mok7zia3pqubmlb3sj5pm8i4bt3g6icl.JPG </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Club C Mid II Revenge Vintage</t>
+          <t>Кроссовки Reebok Classic Leather Mid GTX-Thin</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>11.590.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1f3/296_296_2/erhqtcmroqwyw6ootl4q2bp4soqpbljx.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/eaf/296_296_2/man4efeab6qqovnk4obe172uoy7auz7t.JPG </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Classic Leather Mid GTX-Thin</t>
+          <t>Кроссовки Reebok Zig Kinetica 2.5 Edge Winter</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/79c/296_296_2/mok7zia3pqubmlb3sj5pm8i4bt3g6icl.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/521/296_296_2/rhm0w2q5vrjw01rujx2ue8tmom4zohkn.JPG </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Classic Leather Mid GTX-Thin</t>
+          <t>Кроссовки New Balance 1906R</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>22.990.₽</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/eaf/296_296_2/man4efeab6qqovnk4obe172uoy7auz7t.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/878/296_296_2/koi3s0qa9kfada2kua5gn0d41e5of264.JPG </t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Zig Kinetica 2.5 Edge Winter</t>
+          <t>Кроссовки New Balance 1906R</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>17.990.₽</t>
+          <t>24.990.₽</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/521/296_296_2/rhm0w2q5vrjw01rujx2ue8tmom4zohkn.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/550/296_296_2/ln7d28aw9qjevitjgq55fys4ixma3vqr.JPG </t>
         </is>
       </c>
     </row>
@@ -1875,12 +1875,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>22.990.₽</t>
+          <t>23.990.₽</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/878/296_296_2/koi3s0qa9kfada2kua5gn0d41e5of264.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ed9/296_296_2/250ybpwnpc95a4ko80j6t26zsx95asl7.JPG </t>
         </is>
       </c>
     </row>
@@ -1892,12 +1892,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>24.990.₽</t>
+          <t>22.990.₽</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/550/296_296_2/ln7d28aw9qjevitjgq55fys4ixma3vqr.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/897/296_296_2/z8a3jf41ogax8fy1cxk0n4qz61c1g2ks.JPG </t>
         </is>
       </c>
     </row>
@@ -1909,63 +1909,63 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>23.990.₽</t>
+          <t>24.990.₽</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ed9/296_296_2/250ybpwnpc95a4ko80j6t26zsx95asl7.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a6f/296_296_2/u7c70j4wa3gautpbc1ss7il29a8pc528.JPG </t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906R</t>
+          <t>Кроссовки New Balance 1906D</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>22.990.₽</t>
+          <t>29.990.₽</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/897/296_296_2/z8a3jf41ogax8fy1cxk0n4qz61c1g2ks.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bc4/296_296_2/ycajini0d9aj9wr3mola54wt5tfucub2.JPG </t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906R</t>
+          <t>Кроссовки New Balance 2002R</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>24.990.₽</t>
+          <t>26.990.₽</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a6f/296_296_2/u7c70j4wa3gautpbc1ss7il29a8pc528.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/799/296_296_2/c2qprec6hh9s9e8ydty4t3a44385jk1u.JPG </t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906D</t>
+          <t>Кроссовки New Balance 2002R</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>29.990.₽</t>
+          <t>27.990.₽</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bc4/296_296_2/ycajini0d9aj9wr3mola54wt5tfucub2.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/50e/296_296_2/k22v7n8x69fpaz9xeklqvnyv9s328oxv.JPG </t>
         </is>
       </c>
     </row>
@@ -1977,97 +1977,97 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>26.990.₽</t>
+          <t>27.990.₽</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/799/296_296_2/c2qprec6hh9s9e8ydty4t3a44385jk1u.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/459/296_296_2/v8en6105b46py77w2m230gk3jwvs55la.JPG </t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 2002R</t>
+          <t>Кроссовки New Balance 650</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>27.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/50e/296_296_2/k22v7n8x69fpaz9xeklqvnyv9s328oxv.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9b1/296_296_2/e5pun4m7z0czomlgsf8jcu4qg12dt8zq.JPG </t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 2002R</t>
+          <t>Кроссовки New Balance 574</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>27.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/459/296_296_2/v8en6105b46py77w2m230gk3jwvs55la.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/875/296_296_2/8twqq259pj1pnh824hainnk4bj26tnpm.JPG </t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 650</t>
+          <t>Кроссовки Diadora N902</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>11.190.₽</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9b1/296_296_2/e5pun4m7z0czomlgsf8jcu4qg12dt8zq.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8fa/296_296_2/8mxgc8kxi7np8hemgieicwxv1iij1voo.JPG </t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 574</t>
+          <t>Кроссовки Diadora Camaro</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>8.190.₽</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/875/296_296_2/8twqq259pj1pnh824hainnk4bj26tnpm.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/4fc/296_296_2/srjdigdfxudh215w70x0o8fc8l116xtv.JPG </t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N902</t>
+          <t>Кроссовки PUMA Slipstream Ith</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11.190.₽</t>
+          <t>10.990.₽</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8fa/296_296_2/8mxgc8kxi7np8hemgieicwxv1iij1voo.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/24e/296_296_2/0mc2kmrb9e1lnb1pd33208a0txdd065m.jpg </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
problems resolved, new category added
</commit_message>
<xml_diff>
--- a/sneakers.xlsx
+++ b/sneakers.xlsx
@@ -442,993 +442,993 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
+          <t>Кроссовки Nike Dunk Low</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21.490.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/046/296_296_2/nfeq0doxq94c7x5jnrrzyrrnckknwqqq.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/569/296_296_2/kiaykp1bzsyl6qpj35wzct7yp9zmmk33.JPG </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
+          <t>Кроссовки Nike Air Force 1 '07 LV8</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>21.490.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d95/296_296_2/4j1dbggpomuzyep5g205k53ctzw49ss4.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1e4/296_296_2/y1f68cyora2kci2qmrau9fjjsz9r3309.JPG </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow 5000</t>
+          <t>Кроссовки Nike Air Force 1 '07 LV8 EMB</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/676/296_296_2/th9pk1w9xbr4349gsjsu58xpeqe305xa.jpg </t>
+          <t>https://sneakerhead.ru//upload/resize_cache/iblock/f8f/296_296_2/</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow 6000</t>
+          <t>Кроссовки Jordan 1 Mid</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7f5/296_296_2/fl6dru8cv1ax0w0s3woiegss1e03537y.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b0e/296_296_2/ijozowvq19fs1ds67dd51vkyinpz0v3k.JPG </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow 6000</t>
+          <t>Кроссовки Nike ACG Lowcate</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>14.990.₽</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/008/296_296_2/v2vf86dvtzc50bhbakhk1wgmkpm0d5qw.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/000/296_296_2/iu8erfjqr00ohoui3nq8uzlhkx10gtaw.JPG </t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow 6000</t>
+          <t>Кроссовки Nike Air Max 1 PRM</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17.600.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a13/296_296_2/ylzxac88e18cbc6fdb14lv9pjeos90io.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/3d0/296_296_2/x010tin4ewx9boh08hzmt1qmr8b2licl.JPG </t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow 6000</t>
+          <t>Кроссовки Nike Dunk Low Retro PRM</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18.900.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae3/296_296_2/lk7cjjtlwenbsnaz8lupawb1gg92u89d.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/4b0/296_296_2/zbh1ls7bydwt3hjy9ct4o1tyrhh7268f.JPG </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Jazz 81</t>
+          <t>Кроссовки Jordan 1 Mid</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>13.900.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/346/296_296_2/m9br8zd2ifkgceufr7wgb57ijdvev81w.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/6b0/296_296_2/jtszxm27r6l4nc3jn7gt3b5c93zc8hbb.JPG </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony Shadow Original</t>
+          <t>Кроссовки Jordan 1 High Element Gore-Tex</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>14.400.₽</t>
+          <t>32.000.₽</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/88a/296_296_2/xq8k79ozpfybxo7zfftkj8kbxchw2u4g.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/627/296_296_2/gh7zsvf207s6odnv9wfpft5q36fxm9c4.jpg </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Кроссовки Saucony 3D Grid Hurricane</t>
+          <t>Кроссовки Nike Dunk Low Retro</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17.990.₽</t>
+          <t>24.000.₽</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae1/296_296_2/d8aurlto7sc2me0heb4jmwgbuapecfwl.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b70/296_296_2/qld154oi5icive9kkdj9xm7m3qkffod0.jpg </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Zoom Spiridon Cage 2</t>
+          <t>Кроссовки Nike WMNS Dunk Low</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>24.000.₽</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5e7/296_296_2/t10f9zno250mzry3e6tzpporrk19pxer.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/50f/296_296_2/gjjeedmwrk5o1yprrzl7ilr9p23lhbwg.jpg </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Space Hippie 01</t>
+          <t>Кроссовки New Balance 550</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12.990.₽</t>
+          <t>19.000.₽</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/4f2/296_296_2/12uei3kk0sftwwxxc6era6nh0bhmk5te.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fee/296_296_2/am6089d2oguxveg0welsjhyz306ie7dp.jpg </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 3 Retro</t>
+          <t>Кроссовки Nike Dunk Low Retro</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>30.990.₽</t>
+          <t>21.000.₽</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://sneakerhead.ru//upload/resize_cache/iblock/0ea/296_296_2/yerubilnpprqbqg</t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/3dd/296_296_2/3ao3bblwhi8ewzbq7soeh83q3srdhhaz.JPG </t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Club C BULC</t>
+          <t xml:space="preserve">Кроссовки Jordan 1 Retro High OG </t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>12.490.₽</t>
+          <t>32.000.₽</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ddb/296_296_2/tjy5e9aw7xtp416sxnovl8oxhau81kb1.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/291/296_296_2/6z9elt6nt620izhswytnkd17huwm9fyk.jpg </t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Teveris Nitro</t>
+          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>9.490.₽</t>
+          <t>21.490.₽</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9d3/296_296_2/a88zusqngf1pqwont4j6eq8gh6n0u4tr.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/046/296_296_2/nfeq0doxq94c7x5jnrrzyrrnckknwqqq.JPG </t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Suede</t>
+          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10.190.₽</t>
+          <t>21.490.₽</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c9c/296_296_2/il8snd570s5gmaqisbsozgxc9wnszicy.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d95/296_296_2/4j1dbggpomuzyep5g205k53ctzw49ss4.JPG </t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 13 Retro</t>
+          <t>Кроссовки Saucony Shadow 5000</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>26.990.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1ac/296_296_2/j6w64b3qyc2h086fdv0tsoelza0x1bb8.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/676/296_296_2/th9pk1w9xbr4349gsjsu58xpeqe305xa.jpg </t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 '07</t>
+          <t>Кроссовки Saucony Shadow 6000</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>19.900.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/3ff/296_296_2/3ff05c0b0ca00e50a11d9043f0233cf4.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/7f5/296_296_2/fl6dru8cv1ax0w0s3woiegss1e03537y.JPG </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 High OG QS</t>
+          <t>Кроссовки Saucony Shadow 6000</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bb3/296_296_2/m2t337wcsv54e89oqpij9k29iutwb2qu.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/008/296_296_2/v2vf86dvtzc50bhbakhk1wgmkpm0d5qw.JPG </t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan WMNS 1 Mid</t>
+          <t>Кроссовки Saucony Shadow 6000</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21.990.₽</t>
+          <t>17.600.₽</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/274/296_296_2/27443d085d6096b2f951a9d40f4c669c.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a13/296_296_2/ylzxac88e18cbc6fdb14lv9pjeos90io.JPG </t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 574</t>
+          <t>Кроссовки Saucony Shadow 6000</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>18.900.₽</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fe1/296_296_2/hxbjvb19wez1ka68d1l20c6iu3rv4esj.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae3/296_296_2/lk7cjjtlwenbsnaz8lupawb1gg92u89d.JPG </t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 574</t>
+          <t>Кроссовки Saucony Jazz 81</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>13.900.₽</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c7d/296_296_2/u2f3uguex22a6i36dhd8nfrgm9gkd1kd.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/346/296_296_2/m9br8zd2ifkgceufr7wgb57ijdvev81w.JPG </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Dunk Low Retro</t>
+          <t>Кроссовки Saucony Shadow Original</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>14.400.₽</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/57d/296_296_2/57d1ef7f67047d6aa549245f00fd59a0.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/88a/296_296_2/xq8k79ozpfybxo7zfftkj8kbxchw2u4g.JPG </t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Wave Rider 1</t>
+          <t>Кроссовки Saucony 3D Grid Hurricane</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>18.490.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e7d/296_296_2/d2kcnhpvwxoqjkz029be3ybk5b5bf0fn.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae1/296_296_2/d8aurlto7sc2me0heb4jmwgbuapecfwl.JPG </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Contender</t>
+          <t>Кроссовки Nike Air Zoom Spiridon Cage 2</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b8/296_296_2/fo0qlr2vot0iycmapaark2vd7a43mm5g.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5e7/296_296_2/t10f9zno250mzry3e6tzpporrk19pxer.JPG </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA RS-X Hi</t>
+          <t>Кроссовки Nike Space Hippie 01</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>15.990.₽</t>
+          <t>12.990.₽</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c51/296_296_2/4bpayspdv4t889e9h2xyu5nxfns88p1u.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/4f2/296_296_2/12uei3kk0sftwwxxc6era6nh0bhmk5te.JPG </t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 Shadow</t>
+          <t>Кроссовки Nike Air Force 1 '07 LV8</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cea/296_296_2/ypo43ssbkl0lb9h9pftwjye1cjxahs3c.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/663/296_296_2/tqg36ogeibeejpt48jkcvphr16k4pwgm.JPG </t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 2002R</t>
+          <t>Кроссовки Jordan 3 Retro</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>22.990.₽</t>
+          <t>30.990.₽</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e4d/296_296_2/e4d5b3596faee2bd476db4f711f10cd0.jpg </t>
+          <t>https://sneakerhead.ru//upload/resize_cache/iblock/0ea/296_296_2/yerubilnpprqbqg</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Hi Xtreme Cordura</t>
+          <t>Кроссовки Reebok Club C BULC</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>12.490.₽</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e7c/296_296_2/tnk0n8vldc4nya4fal6nd6eo1aquj1p1.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ddb/296_296_2/tjy5e9aw7xtp416sxnovl8oxhau81kb1.JPG </t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Hi Xtreme Cordura</t>
+          <t>Кроссовки PUMA Teveris Nitro</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>9.490.₽</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cef/296_296_2/obiyh0ljm0v21pz2pp2nxdxv8p6ms6p2.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9d3/296_296_2/a88zusqngf1pqwont4j6eq8gh6n0u4tr.JPG </t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Hi Xtreme</t>
+          <t>Кроссовки PUMA Slipstream Suede</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>10.190.₽</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/72b/296_296_2/j1zj2c90bn9qjq4xx157njfg7fwzx8e1.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c9c/296_296_2/il8snd570s5gmaqisbsozgxc9wnszicy.JPG </t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Кроссовки ASICS Gel-1130</t>
+          <t>Кроссовки Jordan 13 Retro</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14.990.₽</t>
+          <t>26.990.₽</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cfb/296_296_2/k2wlfll8x9rlxb1jz9tp0b8laq83ssw6.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1ac/296_296_2/j6w64b3qyc2h086fdv0tsoelza0x1bb8.JPG </t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Кроссовки ASICS Gel-Kayano 14</t>
+          <t>Кроссовки Nike WMNS Air Force 1 High OG QS</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>21.990.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/822/296_296_2/n8jmzs7zactks5jg11yq4aaq2auup486.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bb3/296_296_2/m2t337wcsv54e89oqpij9k29iutwb2qu.JPG </t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Кроссовки ASICS Gel-Sonoma 15-50</t>
+          <t>Кроссовки Jordan WMNS 1 Mid</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>21.990.₽</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b31/296_296_2/xdqk06l4q6zkuw00ezss8ok1339feeai.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/274/296_296_2/27443d085d6096b2f951a9d40f4c669c.jpg </t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Кроссовки ASICS Gel-Lyte III OG</t>
+          <t>Кроссовки New Balance 574</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>17.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/86c/296_296_2/p0rh90mco2ntvn6gl2s5141v7qrkvdil.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c7d/296_296_2/u2f3uguex22a6i36dhd8nfrgm9gkd1kd.JPG </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Zig Kinetica 2.5 Edge Winter</t>
+          <t>Кроссовки Nike Dunk Low Retro</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>17.990.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/61f/296_296_2/42r6y6lgva4e9z9893t2og2pbd69d20j.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/57d/296_296_2/57d1ef7f67047d6aa549245f00fd59a0.jpg </t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Club C BULC</t>
+          <t>Кроссовки Mizuno Wave Rider 1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>12.690.₽</t>
+          <t>18.490.₽</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/97c/296_296_2/odjm4zj7g4f8izj94e4n7twhdxenmj1g.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e7d/296_296_2/d2kcnhpvwxoqjkz029be3ybk5b5bf0fn.JPG </t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Zoomx Vaporfly Next% 2</t>
+          <t>Кроссовки Mizuno Contender</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>31.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8ec/296_296_2/n1jhzp434z73l3cpbbllz7tzqnl30d09.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b8/296_296_2/fo0qlr2vot0iycmapaark2vd7a43mm5g.JPG </t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Zoomx Vaporfly Next% HKNE</t>
+          <t>Кроссовки PUMA RS-X Hi</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>30.990.₽</t>
+          <t>15.990.₽</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/527/296_296_2/4vwh2jrfl5ggwba5igbszthur2riarok.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c51/296_296_2/4bpayspdv4t889e9h2xyu5nxfns88p1u.jpg </t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Vapormax 2021 FK</t>
+          <t>Кроссовки Nike WMNS Air Force 1 Shadow</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>20.990.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0bd/296_296_2/z50ayuan1ca9kh9x2u0z5soyku823gf1.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cea/296_296_2/ypo43ssbkl0lb9h9pftwjye1cjxahs3c.JPG </t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 Crater Flyknit NN</t>
+          <t>Кроссовки New Balance 2002R</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>22.990.₽</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0c5/296_296_2/2d8fok2200a1b6zimxx29ttp6p1n22zs.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e4d/296_296_2/e4d5b3596faee2bd476db4f711f10cd0.jpg </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кроссовки Jordan 1 Retro High Utility SP </t>
+          <t>Кроссовки PUMA Slipstream Hi Xtreme Cordura</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>24.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9c2/296_296_2/sko9wgbqdrwub5gikyu2to2dg6dn4ihl.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e7c/296_296_2/tnk0n8vldc4nya4fal6nd6eo1aquj1p1.JPG </t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Кроссовки Nike ZoomX Vaporfly</t>
+          <t>Кроссовки PUMA Slipstream Hi Xtreme Cordura</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>31.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a7d/296_296_2/3shqdya6m5ag7frpr4zbt60j0848d46f.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cef/296_296_2/obiyh0ljm0v21pz2pp2nxdxv8p6ms6p2.JPG </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 ZOOM AIR CMFT</t>
+          <t>Кроссовки PUMA Slipstream Hi Xtreme</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>21.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/801/296_296_2/abnpm41gq4kb5d4rwl567px608bfqxy5.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/72b/296_296_2/j1zj2c90bn9qjq4xx157njfg7fwzx8e1.JPG </t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Max SC</t>
+          <t>Кроссовки ASICS Gel-1130</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>14.990.₽</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/045/296_296_2/hda9q0wyrbhni95yqjerddwjzkvcsyi9.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/cfb/296_296_2/k2wlfll8x9rlxb1jz9tp0b8laq83ssw6.JPG </t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Кроссовки Li-Ning Wave Pro</t>
+          <t>Кроссовки ASICS Gel-Kayano 14</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>10.490.₽</t>
+          <t>21.990.₽</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/822/296_296_2/r4pt14oz9i2g99aslvj4kjvmyxaohosr.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/822/296_296_2/n8jmzs7zactks5jg11yq4aaq2auup486.JPG </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Кроссовки Li-Ning Wave Pro SE</t>
+          <t>Кроссовки ASICS Gel-Sonoma 15-50</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>11.590.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0e4/296_296_2/baf4l4w7rtki2j50r36bvmtnxszrt14e.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b31/296_296_2/xdqk06l4q6zkuw00ezss8ok1339feeai.JPG </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Кроссовки Nike ACG Moc 3.5</t>
+          <t>Кроссовки ASICS Gel-Lyte III OG</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>11.990.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/60f/296_296_2/xbv1uldhbv70yh7k990nhwv25643u62k.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/86c/296_296_2/p0rh90mco2ntvn6gl2s5141v7qrkvdil.JPG </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 LE (GS)</t>
+          <t>Кроссовки Reebok Zig Kinetica 2.5 Edge Winter</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d5e/296_296_2/d5ebbacaa03f8ce6957fbab928d42eee.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/61f/296_296_2/42r6y6lgva4e9z9893t2og2pbd69d20j.JPG </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan WMNS 1 Acclimate</t>
+          <t>Кроссовки Reebok Club C BULC</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>21.000.₽</t>
+          <t>12.690.₽</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/510/296_296_2/3mencgkhigsy0rp4az1030oxwmt3zsdu.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/97c/296_296_2/odjm4zj7g4f8izj94e4n7twhdxenmj1g.JPG </t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan WMNS 1 Acclimate</t>
+          <t>Кроссовки Nike Zoomx Vaporfly Next% 2</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>21.000.₽</t>
+          <t>31.990.₽</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fa7/296_296_2/6u4o87au7d6veyqbjx5lu168ckgspwxx.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8ec/296_296_2/n1jhzp434z73l3cpbbllz7tzqnl30d09.JPG </t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan WMNS 1 Acclimate</t>
+          <t>Кроссовки Nike Zoomx Vaporfly Next% HKNE</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>21.000.₽</t>
+          <t>30.990.₽</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a1c/296_296_2/yo8n34xfiwo8s6arqiln0owrq0i80iba.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/527/296_296_2/4vwh2jrfl5ggwba5igbszthur2riarok.JPG </t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
+          <t>Кроссовки Nike WMNS Air Vapormax 2021 FK</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>20.000.₽</t>
+          <t>20.990.₽</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fcf/296_296_2/fsokqf6rdx7ohynq1ynvzy72iub42dc6.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0bd/296_296_2/z50ayuan1ca9kh9x2u0z5soyku823gf1.JPG </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 '07</t>
+          <t>Кроссовки Nike ZoomX Vaporfly</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>31.990.₽</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/2d5/296_296_2/1q2tek49apdlbtc6ggsj3h39zono0giv.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a7d/296_296_2/3shqdya6m5ag7frpr4zbt60j0848d46f.JPG </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
+          <t>Кроссовки Jordan 1 ZOOM AIR CMFT</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>21.990.₽</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a3a/296_296_2/nmivl13a5m0cy447mnyt9xy2c6i3d13w.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/801/296_296_2/abnpm41gq4kb5d4rwl567px608bfqxy5.JPG </t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Air Force 1 '07</t>
+          <t>Кроссовки Li-Ning Wave Pro</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>10.490.₽</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/5b2/296_296_2/fpbnqjfiyl6u8yvf42agnoknzgk1yg0m.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/822/296_296_2/r4pt14oz9i2g99aslvj4kjvmyxaohosr.JPG </t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Кроссовки Nike Dunk Low Retro PRM</t>
+          <t>Кроссовки Li-Ning Wave Pro SE</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>20.990.₽</t>
+          <t>11.590.₽</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/483/296_296_2/5ckjgio7rfyerf2s9ek5y6wuba9a0h01.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/0e4/296_296_2/baf4l4w7rtki2j50r36bvmtnxszrt14e.JPG </t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Кроссовки Nike WMNS Dunk Low LX</t>
+          <t>Кроссовки Nike ACG Moc 3.5</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>17.990.₽</t>
+          <t>11.990.₽</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/47f/296_296_2/tbrur5tjllknu907e8r62eadzohmecdq.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/60f/296_296_2/xbv1uldhbv70yh7k990nhwv25643u62k.JPG </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Кроссовки Nike ACG Mountain Fly 2 Low</t>
+          <t>Кроссовки Nike Air Force 1 LE (GS)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1438,422 +1438,422 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/da4/296_296_2/o1swj5riifulqv62i7x7yag0esds6tlb.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d5e/296_296_2/d5ebbacaa03f8ce6957fbab928d42eee.jpg </t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Suede</t>
+          <t>Кроссовки Jordan WMNS 1 Acclimate</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>10.190.₽</t>
+          <t>21.000.₽</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1e7/296_296_2/luq43cv83p432jwj3zolpe8ttvqronqh.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/510/296_296_2/3mencgkhigsy0rp4az1030oxwmt3zsdu.JPG </t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N9000 Rally Giulietta Itali</t>
+          <t>Кроссовки Jordan WMNS 1 Acclimate</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>26.790.₽</t>
+          <t>21.000.₽</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/998/296_296_2/prlbuactqqt6km4sn7r8snysz9sl53ik.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fa7/296_296_2/6u4o87au7d6veyqbjx5lu168ckgspwxx.JPG </t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora B.560 Used</t>
+          <t>Кроссовки Jordan WMNS 1 Acclimate</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>24.490.₽</t>
+          <t>21.000.₽</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c64/296_296_2/c0fqcfk3ssgfnrxll76psxi33uyvn813.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a1c/296_296_2/yo8n34xfiwo8s6arqiln0owrq0i80iba.JPG </t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora B.56 Icona</t>
+          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>12.190.₽</t>
+          <t>20.000.₽</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/155/296_296_2/tjwnrwrow86mujignvqhapmy0wdvc56f.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/fcf/296_296_2/fsokqf6rdx7ohynq1ynvzy72iub42dc6.JPG </t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora Magic Basket Low Suede Leather</t>
+          <t>Кроссовки Nike Air Force 1 '07</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>12.590.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/85a/296_296_2/ifh2xgzc3lkvi4l919fjdgqbvgmkf1sn.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/2d5/296_296_2/1q2tek49apdlbtc6ggsj3h39zono0giv.JPG </t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N.92 Advance</t>
+          <t>Кроссовки Nike WMNS Air Force 1 '07 LX</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>10.490.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d00/296_296_2/2o731rmeir6av9x2i70txdm46dqoz0xx.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a3a/296_296_2/nmivl13a5m0cy447mnyt9xy2c6i3d13w.JPG </t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N902 Hairy Suede</t>
+          <t>Кроссовки Nike Air Force 1 '07</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>11.190.₽</t>
+          <t>19.990.₽</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/3da/296_296_2/91pw2xy60tn25sp2t0qse7leuzppif85.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8d6/296_296_2/1s2e120rrbes2jetcimmpvd82pmkvn93.JPG </t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N902</t>
+          <t>Кроссовки Nike WMNS Dunk Low LX</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>14.890.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1c9/296_296_2/wej9c1s9undfcvlxl3jwoh6kb6funvxu.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/47f/296_296_2/tbrur5tjllknu907e8r62eadzohmecdq.JPG </t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora V7000 Winter</t>
+          <t>Кроссовки Nike ACG Mountain Fly 2 Low</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>14.190.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae4/296_296_2/fnt7nsc3jupi22ue464cxbp9jmwbqq20.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/da4/296_296_2/o1swj5riifulqv62i7x7yag0esds6tlb.JPG </t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t xml:space="preserve">Кроссовки Diadora V7000 Winter </t>
+          <t>Кроссовки PUMA Slipstream Suede</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>14.190.₽</t>
+          <t>10.190.₽</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e69/296_296_2/3urr2nxltn6nrnog4mqhliulquiy7p97.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1e7/296_296_2/luq43cv83p432jwj3zolpe8ttvqronqh.JPG </t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N9002 Winter</t>
+          <t>Кроссовки Diadora N9000 Rally Giulietta Itali</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16.390.₽</t>
+          <t>26.790.₽</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e65/296_296_2/4fe7jsy4klih38kzyqe8labyt2wys8ar.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/998/296_296_2/prlbuactqqt6km4sn7r8snysz9sl53ik.JPG </t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N9002 Winter</t>
+          <t>Кроссовки Diadora B.560 Used</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16.390.₽</t>
+          <t>24.490.₽</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/688/296_296_2/47achzhjvpul8jbeyn5pf26qubzwmuf8.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c64/296_296_2/c0fqcfk3ssgfnrxll76psxi33uyvn813.JPG </t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Contender</t>
+          <t>Кроссовки Diadora B.56 Icona</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16.990.₽</t>
+          <t>12.190.₽</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b56/296_296_2/ce779p9n380lfnw58yk8b1han4ftjbwc.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/155/296_296_2/tjwnrwrow86mujignvqhapmy0wdvc56f.JPG </t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Wave Rider 10</t>
+          <t>Кроссовки Diadora Magic Basket Low Suede Leather</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>20.990.₽</t>
+          <t>12.590.₽</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/2a8/296_296_2/2f7yvxz0a9pvzapkmhkca97lgawh4amx.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/85a/296_296_2/ifh2xgzc3lkvi4l919fjdgqbvgmkf1sn.JPG </t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno City Wind</t>
+          <t>Кроссовки Diadora N.92 Advance</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>14.990.₽</t>
+          <t>10.490.₽</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c8e/296_296_2/k9sjc434r3qmn6my5dwwjz325mwxzeh0.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/d00/296_296_2/2o731rmeir6av9x2i70txdm46dqoz0xx.JPG </t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Wave Mujin TL GTX</t>
+          <t>Кроссовки Diadora N902 Hairy Suede</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>24.990.₽</t>
+          <t>11.190.₽</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/396/296_296_2/4a57232ajluzciuvomuvow2xc4p4vzn2.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/3da/296_296_2/91pw2xy60tn25sp2t0qse7leuzppif85.JPG </t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Кроссовки Mizuno Wave Mujin TL GTX</t>
+          <t>Кроссовки Diadora N902</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>24.990.₽</t>
+          <t>14.890.₽</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/f37/296_296_2/9qo14d029kjb0nri86pwhug41db3wjmg.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1c9/296_296_2/wej9c1s9undfcvlxl3jwoh6kb6funvxu.JPG </t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
+          <t>Кроссовки Diadora V7000 Winter</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>20.000.₽</t>
+          <t>14.190.₽</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1d0/296_296_2/5y0m14acunvwl6ch0y16y4c7vytgvayd.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ae4/296_296_2/fnt7nsc3jupi22ue464cxbp9jmwbqq20.jpg </t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
+          <t xml:space="preserve">Кроссовки Diadora V7000 Winter </t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>24.000.₽</t>
+          <t>14.190.₽</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/955/296_296_2/04i3rsojwt4rs4hxrhwbzawyj52zyti3.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e69/296_296_2/3urr2nxltn6nrnog4mqhliulquiy7p97.JPG </t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Club C Mid II Revenge Vintage</t>
+          <t>Кроссовки Diadora N9002 Winter</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>11.590.₽</t>
+          <t>16.390.₽</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1f3/296_296_2/erhqtcmroqwyw6ootl4q2bp4soqpbljx.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/e65/296_296_2/4fe7jsy4klih38kzyqe8labyt2wys8ar.JPG </t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Classic Leather Mid GTX-Thin</t>
+          <t>Кроссовки Diadora N9002 Winter</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>16.390.₽</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/79c/296_296_2/mok7zia3pqubmlb3sj5pm8i4bt3g6icl.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/688/296_296_2/47achzhjvpul8jbeyn5pf26qubzwmuf8.JPG </t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Classic Leather Mid GTX-Thin</t>
+          <t>Кроссовки Mizuno Contender</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>18.990.₽</t>
+          <t>16.990.₽</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/eaf/296_296_2/man4efeab6qqovnk4obe172uoy7auz7t.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/b56/296_296_2/ce779p9n380lfnw58yk8b1han4ftjbwc.JPG </t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Кроссовки Reebok Zig Kinetica 2.5 Edge Winter</t>
+          <t>Кроссовки Mizuno Wave Rider 10</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>17.990.₽</t>
+          <t>20.990.₽</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/521/296_296_2/rhm0w2q5vrjw01rujx2ue8tmom4zohkn.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/2a8/296_296_2/2f7yvxz0a9pvzapkmhkca97lgawh4amx.JPG </t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906R</t>
+          <t>Кроссовки Mizuno City Wind</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>22.990.₽</t>
+          <t>14.990.₽</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/878/296_296_2/koi3s0qa9kfada2kua5gn0d41e5of264.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/c8e/296_296_2/k9sjc434r3qmn6my5dwwjz325mwxzeh0.JPG </t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906R</t>
+          <t>Кроссовки Mizuno Wave Mujin TL GTX</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1863,211 +1863,211 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/550/296_296_2/ln7d28aw9qjevitjgq55fys4ixma3vqr.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/396/296_296_2/4a57232ajluzciuvomuvow2xc4p4vzn2.JPG </t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906R</t>
+          <t>Кроссовки Mizuno Wave Mujin TL GTX</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>23.990.₽</t>
+          <t>24.990.₽</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ed9/296_296_2/250ybpwnpc95a4ko80j6t26zsx95asl7.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/f37/296_296_2/9qo14d029kjb0nri86pwhug41db3wjmg.JPG </t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906R</t>
+          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>22.990.₽</t>
+          <t>20.000.₽</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/897/296_296_2/z8a3jf41ogax8fy1cxk0n4qz61c1g2ks.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1d0/296_296_2/5y0m14acunvwl6ch0y16y4c7vytgvayd.jpg </t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906R</t>
+          <t>Кроссовки Jordan 1 Mid SE (GS)</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>24.990.₽</t>
+          <t>24.000.₽</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a6f/296_296_2/u7c70j4wa3gautpbc1ss7il29a8pc528.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/955/296_296_2/04i3rsojwt4rs4hxrhwbzawyj52zyti3.jpg </t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 1906D</t>
+          <t>Кроссовки Reebok Club C Mid II Revenge Vintage</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>29.990.₽</t>
+          <t>11.590.₽</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bc4/296_296_2/ycajini0d9aj9wr3mola54wt5tfucub2.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/1f3/296_296_2/erhqtcmroqwyw6ootl4q2bp4soqpbljx.JPG </t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 2002R</t>
+          <t>Кроссовки Reebok Classic Leather Mid GTX-Thin</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>26.990.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/799/296_296_2/c2qprec6hh9s9e8ydty4t3a44385jk1u.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/79c/296_296_2/mok7zia3pqubmlb3sj5pm8i4bt3g6icl.JPG </t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 2002R</t>
+          <t>Кроссовки Reebok Classic Leather Mid GTX-Thin</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>27.990.₽</t>
+          <t>18.990.₽</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/50e/296_296_2/k22v7n8x69fpaz9xeklqvnyv9s328oxv.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/eaf/296_296_2/man4efeab6qqovnk4obe172uoy7auz7t.JPG </t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 2002R</t>
+          <t>Кроссовки Reebok Zig Kinetica 2.5 Edge Winter</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>27.990.₽</t>
+          <t>17.990.₽</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/459/296_296_2/v8en6105b46py77w2m230gk3jwvs55la.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/521/296_296_2/rhm0w2q5vrjw01rujx2ue8tmom4zohkn.JPG </t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 650</t>
+          <t>Кроссовки New Balance 1906R</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>22.990.₽</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/9b1/296_296_2/e5pun4m7z0czomlgsf8jcu4qg12dt8zq.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/878/296_296_2/koi3s0qa9kfada2kua5gn0d41e5of264.JPG </t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Кроссовки New Balance 574</t>
+          <t>Кроссовки New Balance 1906R</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>19.990.₽</t>
+          <t>24.990.₽</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/875/296_296_2/8twqq259pj1pnh824hainnk4bj26tnpm.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/550/296_296_2/ln7d28aw9qjevitjgq55fys4ixma3vqr.JPG </t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora N902</t>
+          <t>Кроссовки New Balance 1906R</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>11.190.₽</t>
+          <t>23.990.₽</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/8fa/296_296_2/8mxgc8kxi7np8hemgieicwxv1iij1voo.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/ed9/296_296_2/250ybpwnpc95a4ko80j6t26zsx95asl7.JPG </t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Кроссовки Diadora Camaro</t>
+          <t>Кроссовки New Balance 1906R</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>8.190.₽</t>
+          <t>24.990.₽</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/4fc/296_296_2/srjdigdfxudh215w70x0o8fc8l116xtv.JPG </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/a6f/296_296_2/u7c70j4wa3gautpbc1ss7il29a8pc528.JPG </t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Кроссовки PUMA Slipstream Ith</t>
+          <t>Кроссовки New Balance 1906D</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>10.990.₽</t>
+          <t>29.990.₽</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/24e/296_296_2/0mc2kmrb9e1lnb1pd33208a0txdd065m.jpg </t>
+          <t xml:space="preserve">https://sneakerhead.ru//upload/resize_cache/iblock/bc4/296_296_2/ycajini0d9aj9wr3mola54wt5tfucub2.JPG </t>
         </is>
       </c>
     </row>

</xml_diff>